<commit_message>
Add API list, reference docs
</commit_message>
<xml_diff>
--- a/docs/02_requirements/nfr (v2).xlsx
+++ b/docs/02_requirements/nfr (v2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Farheen\OBE-TRACKING-SYSTEM\docs\02_requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01698B4D-EE67-4E25-A664-2FF0956E651D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0409DBB2-E802-470E-8409-8C4028627AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>1. Performance</t>
   </si>
@@ -57,36 +57,9 @@
     <t>8. Availability</t>
   </si>
   <si>
-    <t>NFR23. The system shall be accessible through standard web browsers.</t>
-  </si>
-  <si>
-    <t>NFR16. Configuration changes shall not affect previously stored historical data.</t>
-  </si>
-  <si>
-    <t>NFR17. Report formats and survey questions shall be updatable without impacting existing data.</t>
-  </si>
-  <si>
     <t>6. Scalability and Extensibility</t>
   </si>
   <si>
-    <t>NFR18. The system design shall support addition of new departments, programs, or courses in the future.</t>
-  </si>
-  <si>
-    <t>NFR19. The system shall allow addition of new survey types or indirect assessment tools without redesigning the system.</t>
-  </si>
-  <si>
-    <t>NFR20. The system shall maintain audit logs for key actions such as data entry, edits, approvals, and report verification.</t>
-  </si>
-  <si>
-    <t>NFR21. Audit logs shall be protected from unauthorized modification and viewable only by authorized roles.</t>
-  </si>
-  <si>
-    <t>NFR22. Generated reports shall be suitable for accreditation and academic audit purposes.</t>
-  </si>
-  <si>
-    <t>NFR24. System maintenance activities shall not affect the integrity of stored academic and survey data.</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -181,6 +154,60 @@
   </si>
   <si>
     <t>Targets, thresholds, weightages, and survey configurations shall be configurable without changing source code.</t>
+  </si>
+  <si>
+    <t>Configuration changes shall not affect previously stored historical data.</t>
+  </si>
+  <si>
+    <t>NFR16</t>
+  </si>
+  <si>
+    <t>Report formats and survey questions shall be updatable without impacting existing data.</t>
+  </si>
+  <si>
+    <t>NFR17</t>
+  </si>
+  <si>
+    <t>The system design shall support addition of new departments, programs, or courses in the future.</t>
+  </si>
+  <si>
+    <t>The system shall allow addition of new survey types or indirect assessment tools without redesigning the system.</t>
+  </si>
+  <si>
+    <t>NFR18</t>
+  </si>
+  <si>
+    <t>NFR19</t>
+  </si>
+  <si>
+    <t>The system shall maintain audit logs for key actions such as data entry, edits, approvals, and report verification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Audit logs shall be protected from unauthorized modification and viewable only by authorized roles.</t>
+  </si>
+  <si>
+    <t>Generated reports shall be suitable for accreditation and academic audit purposes.</t>
+  </si>
+  <si>
+    <t>The system shall be accessible through standard web browsers.</t>
+  </si>
+  <si>
+    <t>System maintenance activities shall not affect the integrity of stored academic and survey data.</t>
+  </si>
+  <si>
+    <t>NFR20</t>
+  </si>
+  <si>
+    <t>NFR21</t>
+  </si>
+  <si>
+    <t>NFR22</t>
+  </si>
+  <si>
+    <t>NFR23</t>
+  </si>
+  <si>
+    <t>NFR24</t>
   </si>
 </sst>
 </file>
@@ -188,9 +215,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;NFR &quot;#"/>
+    <numFmt numFmtId="164" formatCode="&quot;NFR &quot;#"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +231,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -213,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -221,16 +264,230 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,271 +768,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="9" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>16</v>
-      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B19:I19"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>